<commit_message>
Before making second migrations (adding exam length, linking to User, and other changes)
</commit_message>
<xml_diff>
--- a/other/logic map.xlsx
+++ b/other/logic map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/326d2f4c0460448a/Web Dev Projects/proj1_proctorx/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A2072F8-BDB7-43C0-83D3-2654F926774E}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{335DF048-ABD9-4882-9512-043357963215}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>What do I need?</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Homepage</t>
   </si>
   <si>
-    <t>Content - Homepage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Link - Take exam </t>
-  </si>
-  <si>
     <t xml:space="preserve">Link - Help Centre </t>
   </si>
   <si>
@@ -66,18 +60,9 @@
     <t xml:space="preserve">Page - Homepage </t>
   </si>
   <si>
-    <t>Page - Login page</t>
-  </si>
-  <si>
-    <t>Form - login</t>
-  </si>
-  <si>
     <t>Page - Help centre</t>
   </si>
   <si>
-    <t>Form - User or instructor registration</t>
-  </si>
-  <si>
     <t>Form - Login</t>
   </si>
   <si>
@@ -90,9 +75,6 @@
     <t>Link - My orders</t>
   </si>
   <si>
-    <t>Content</t>
-  </si>
-  <si>
     <t>Link - Support link</t>
   </si>
   <si>
@@ -256,6 +238,9 @@
   </si>
   <si>
     <t>Session</t>
+  </si>
+  <si>
+    <t>Form - User registration</t>
   </si>
 </sst>
 </file>
@@ -605,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,242 +607,217 @@
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>19</v>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -867,145 +827,145 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reservations.html now shows available reservations
</commit_message>
<xml_diff>
--- a/other/logic map.xlsx
+++ b/other/logic map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/326d2f4c0460448a/Web Dev Projects/proj1_proctorx/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{335DF048-ABD9-4882-9512-043357963215}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2671A8CC-A773-4128-938C-D8E18EA66FC3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>What do I need?</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Link - My sessions</t>
   </si>
   <si>
-    <t>Link - My orders</t>
-  </si>
-  <si>
     <t>Link - Support link</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>GET - Sessions content</t>
   </si>
   <si>
-    <t>GET - Orders</t>
-  </si>
-  <si>
     <t>GET - University exams</t>
   </si>
   <si>
@@ -241,13 +235,22 @@
   </si>
   <si>
     <t>Form - User registration</t>
+  </si>
+  <si>
+    <t>GET - Orders in the cart</t>
+  </si>
+  <si>
+    <t>Link - Cart</t>
+  </si>
+  <si>
+    <t>Delete session</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +272,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -302,10 +319,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -590,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +618,7 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" customWidth="1"/>
@@ -649,7 +668,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -673,23 +692,23 @@
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>20</v>
+      <c r="E20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>15</v>
+      <c r="D21" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>21</v>
+      <c r="E22" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
@@ -698,126 +717,129 @@
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G28" t="s">
+      <c r="G28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G29" t="s">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I31" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G35" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F44" t="s">
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G45" t="s">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I47" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,145 +849,145 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,5 +1002,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added sendgrid function, still working on email templates. Troubleshooting issue with username field
</commit_message>
<xml_diff>
--- a/other/logic map.xlsx
+++ b/other/logic map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/326d2f4c0460448a/Web Dev Projects/proj1_proctorx/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2671A8CC-A773-4128-938C-D8E18EA66FC3}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FFB713C-CA04-479A-9603-CDBD72C3B9C6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,22 +755,22 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on login screen css
</commit_message>
<xml_diff>
--- a/other/logic map.xlsx
+++ b/other/logic map.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/326d2f4c0460448a/Web Dev Projects/proj1_proctorx/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FFB713C-CA04-479A-9603-CDBD72C3B9C6}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0BF6B93-55B7-4534-8420-C998458503CF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>What do I need?</t>
   </si>
@@ -244,6 +245,21 @@
   </si>
   <si>
     <t>Delete session</t>
+  </si>
+  <si>
+    <t>Front end</t>
+  </si>
+  <si>
+    <t>Master template</t>
+  </si>
+  <si>
+    <t>POST request to select reservation</t>
+  </si>
+  <si>
+    <t>Nav</t>
+  </si>
+  <si>
+    <t>Footer</t>
   </si>
 </sst>
 </file>
@@ -281,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,12 +312,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -319,12 +329,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -607,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +751,7 @@
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="H30" s="3" t="s">
@@ -775,22 +784,22 @@
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G39" t="s">
+      <c r="G39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -815,7 +824,7 @@
       </c>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F44" s="2" t="s">
@@ -837,166 +846,191 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2" t="s">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2" t="s">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1004,4 +1038,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6467357D-DB44-464A-A92E-8B05B113E3E3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished public template htmls: login, register, forgot password and set password
</commit_message>
<xml_diff>
--- a/other/logic map.xlsx
+++ b/other/logic map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/326d2f4c0460448a/Web Dev Projects/proj1_proctorx/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0BF6B93-55B7-4534-8420-C998458503CF}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAA47824-AF83-4618-9EA4-7763DD3135A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>What do I need?</t>
   </si>
@@ -250,16 +250,43 @@
     <t>Front end</t>
   </si>
   <si>
-    <t>Master template</t>
-  </si>
-  <si>
     <t>POST request to select reservation</t>
   </si>
   <si>
-    <t>Nav</t>
-  </si>
-  <si>
-    <t>Footer</t>
+    <t>Template 1</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Template 2</t>
+  </si>
+  <si>
+    <t>User sessions</t>
+  </si>
+  <si>
+    <t>User cart</t>
+  </si>
+  <si>
+    <t>Forgot password</t>
+  </si>
+  <si>
+    <t>Password reset</t>
+  </si>
+  <si>
+    <t>Password changed confirmaiton ?</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Shrinking the screen vertically cuts of top content. However bottom content is always available through scroll</t>
   </si>
 </sst>
 </file>
@@ -618,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,29 +873,59 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,14 +1099,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6467357D-DB44-464A-A92E-8B05B113E3E3}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="97.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished payment functionality but broke the cart due to change in css and html - I'll have to get the cart html and css from previous commit
</commit_message>
<xml_diff>
--- a/other/logic map.xlsx
+++ b/other/logic map.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/326d2f4c0460448a/Web Dev Projects/proj1_proctorx/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAA47824-AF83-4618-9EA4-7763DD3135A3}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="11_F25DC773A252ABDACC10486081986F365ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EBC9C99-1F40-481B-BA32-EB1A286B3252}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>What do I need?</t>
   </si>
@@ -287,6 +288,30 @@
   </si>
   <si>
     <t>Shrinking the screen vertically cuts of top content. However bottom content is always available through scroll</t>
+  </si>
+  <si>
+    <t>To-dos</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>ProctorX - About link</t>
+  </si>
+  <si>
+    <t>My Account - Account Settings</t>
+  </si>
+  <si>
+    <t>My Account - Password Settings</t>
+  </si>
+  <si>
+    <t>Resizing to phone size</t>
+  </si>
+  <si>
+    <t>My Orders table format</t>
+  </si>
+  <si>
+    <t>Credit card - submit actions</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6467357D-DB44-464A-A92E-8B05B113E3E3}">
   <dimension ref="B3:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -1128,4 +1153,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139F09B6-C2E6-4681-8431-B7655C08C1A2}">
+  <dimension ref="B3:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>